<commit_message>
Proyecto de conmutacion terminado
</commit_message>
<xml_diff>
--- a/subnetting.xlsx
+++ b/subnetting.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\TercerCuatri\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10320" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>#</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>2024:2:110:0</t>
+  </si>
+  <si>
+    <t>RIP juana</t>
+  </si>
+  <si>
+    <t>Kira 30</t>
+  </si>
+  <si>
+    <t>Fatima 7</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -327,6 +336,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -633,22 +645,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -656,311 +668,326 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2">
+        <v>2046</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2046</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>1022</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1022</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="2">
+        <v>1022</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1022</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="2">
+        <v>1022</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1022</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2">
+        <v>1022</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1022</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2">
+        <v>510</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="2">
-        <v>510</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2">
+        <v>510</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" s="2">
-        <v>510</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2">
+        <v>254</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" s="2">
-        <v>254</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="2">
+        <v>126</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="2">
-        <v>126</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="2">
+        <v>126</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C11" s="2">
-        <v>126</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="2">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="2">
-        <v>62</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>44</v>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>